<commit_message>
Correccionn AltasBatch, Asignacion de Zonas, Llamadas Perdidas)
</commit_message>
<xml_diff>
--- a/src/assets/test.xlsx
+++ b/src/assets/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert.sanchez/Desktop/Angular/cycV5/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert.sanchez/Desktop/Angular/cycV5/src/assets/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB18C1CC-C08C-654D-8390-C01DBDAB3923}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BB1135-E213-7A4C-B8B7-16D82B1C52FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CA8E2AB9-0C40-FD49-B1A0-BAFB652E96EE}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="contratos">Hoja2!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Nombres</t>
   </si>
@@ -64,7 +64,19 @@
     <t>Pais</t>
   </si>
   <si>
-    <t>CO</t>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>Pepito Price</t>
+  </si>
+  <si>
+    <t>José Pepe</t>
+  </si>
+  <si>
+    <t>Price Travel</t>
+  </si>
+  <si>
+    <t>ppprice@gmail.com</t>
   </si>
   <si>
     <t>Contrato</t>
@@ -88,271 +100,10 @@
     <t>Visa</t>
   </si>
   <si>
-    <t>LONDOÑO RAMIREZ</t>
+    <t>Pepita</t>
   </si>
   <si>
-    <t xml:space="preserve">NATALHYA </t>
-  </si>
-  <si>
-    <t>MACCA MENECES</t>
-  </si>
-  <si>
-    <t>NINI JOHANNA</t>
-  </si>
-  <si>
-    <t>VIVAS FORERO </t>
-  </si>
-  <si>
-    <t>DIANA PAOLA</t>
-  </si>
-  <si>
-    <t>ARBOLEDA MIDEROS</t>
-  </si>
-  <si>
-    <t>JHON JAIRO</t>
-  </si>
-  <si>
-    <t>FLOREZ SALCEDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JONNATAN </t>
-  </si>
-  <si>
-    <t>LEAL VARGAS</t>
-  </si>
-  <si>
-    <t>CLAUDIA JOHANA</t>
-  </si>
-  <si>
-    <t>BENITEZ PASTRANA</t>
-  </si>
-  <si>
-    <t>LEIDY JOHANNA</t>
-  </si>
-  <si>
-    <t>SUAZA RODRIGUEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KATERINE </t>
-  </si>
-  <si>
-    <t>AGUIRRE ALFONSO</t>
-  </si>
-  <si>
-    <t>JHON ALEXANDER</t>
-  </si>
-  <si>
-    <t>REYES CORTES</t>
-  </si>
-  <si>
-    <t>CARLOS ANDRES</t>
-  </si>
-  <si>
-    <t>AGUDELO CARDONA</t>
-  </si>
-  <si>
-    <t>DANIEL FELIPE</t>
-  </si>
-  <si>
-    <t>MURCIA DIAZ</t>
-  </si>
-  <si>
-    <t>CRISTIAN ANDRES</t>
-  </si>
-  <si>
-    <t>RAMIREZ VILLEGAS</t>
-  </si>
-  <si>
-    <t>CRYSTIAN JHOAN</t>
-  </si>
-  <si>
-    <t>LONDOÑO CALERO</t>
-  </si>
-  <si>
-    <t>JOSE ANTONIO</t>
-  </si>
-  <si>
-    <t>TIMOTE VILLACI</t>
-  </si>
-  <si>
-    <t>FRANCHESCA ALEJANDRA</t>
-  </si>
-  <si>
-    <t>HURTADO DIAZ</t>
-  </si>
-  <si>
-    <t>MAYRA ALEJANDRA</t>
-  </si>
-  <si>
-    <t>CAMACHO ANAYA</t>
-  </si>
-  <si>
-    <t>JULIETH DAYANA</t>
-  </si>
-  <si>
-    <t>ACEVEDO MEZA</t>
-  </si>
-  <si>
-    <t>JAZMIN TATIANA</t>
-  </si>
-  <si>
-    <t>PEREZ CAMACHO</t>
-  </si>
-  <si>
-    <t>MARIANA KRISBEL</t>
-  </si>
-  <si>
-    <t>SOLANO MENESES</t>
-  </si>
-  <si>
-    <t>DIANA PATRICIA</t>
-  </si>
-  <si>
-    <t>ROJAS ORTIZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YENNIFER </t>
-  </si>
-  <si>
-    <t>LUCUMI CASTRO</t>
-  </si>
-  <si>
-    <t>LINA MARIA</t>
-  </si>
-  <si>
-    <t>Natalnya Londono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shermie104@hotmail.com                                                          </t>
-  </si>
-  <si>
-    <t>Nini Macca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">johannamacca113@gmail.com                                                       </t>
-  </si>
-  <si>
-    <t>Diana Vivas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dalavivasforero@gmail.com                                                       </t>
-  </si>
-  <si>
-    <t>Jhon Arboleda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jhonjairomideros@gmail.com                                                      </t>
-  </si>
-  <si>
-    <t>Jonnatan Florez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jonok721@gmail.com                                                              </t>
-  </si>
-  <si>
-    <t>Claudia Leal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc.comercialcl@gmail.com                                                        </t>
-  </si>
-  <si>
-    <t> Leidy Benitez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cristal3310@hotmail.com                                                         </t>
-  </si>
-  <si>
-    <t>Katerine Suaza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kathe932011@hotmail.com                                                         </t>
-  </si>
-  <si>
-    <t>Jhon Aguirre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aguirrealfon42@hotmail.com                                                      </t>
-  </si>
-  <si>
-    <t>Carlos Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hikarimono91@hotmail.com                                                        </t>
-  </si>
-  <si>
-    <t>Daniel Agudelo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">felo-1991@hotmail.com                                                           </t>
-  </si>
-  <si>
-    <t>Cristian Murcia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">murciac630@gmail.com                                                            </t>
-  </si>
-  <si>
-    <t>Crystian Ramirez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crystianramirez@icloud.com                                                      </t>
-  </si>
-  <si>
-    <t>Jose Calero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jose401524@hotmail.com                                                          </t>
-  </si>
-  <si>
-    <t> Franchesca Timote</t>
-  </si>
-  <si>
-    <t xml:space="preserve">villaci.alejandra@gmail.com                                                     </t>
-  </si>
-  <si>
-    <t>Mayra Hurtado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alejan1565@gmail.com                                                            </t>
-  </si>
-  <si>
-    <t> Julieth Camacho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">julieth.yaya@gmail.com                                                          </t>
-  </si>
-  <si>
-    <t> Jazmin Acevedo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jazminge0814@hotmail.com                                                        </t>
-  </si>
-  <si>
-    <t>Mariana Camacho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marianakrysbel@gmail.com                                                        </t>
-  </si>
-  <si>
-    <t>Diana Solano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dianapatria0391@gmail.com                                                       </t>
-  </si>
-  <si>
-    <t>Yennifer Rojas</t>
-  </si>
-  <si>
-    <t>41001233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yegami101827@gmail.com                                                          </t>
-  </si>
-  <si>
-    <t> Lina Lucumi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imlucumi@hotmail.com                                                            </t>
+    <t>Pepita Price</t>
   </si>
 </sst>
 </file>
@@ -362,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -394,30 +145,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -459,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -471,22 +205,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -803,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6EF1D2-C469-BC4B-AD1F-1E217E15B092}">
-  <dimension ref="A1:O880"/>
+  <dimension ref="A1:O901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,8 +533,7 @@
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="26.5" customWidth="1"/>
     <col min="11" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
@@ -855,882 +572,242 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>16</v>
+      <c r="D2">
+        <v>49600123</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
+      <c r="E2">
+        <v>123123123</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>19</v>
+      <c r="F2" s="1">
+        <v>43320</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>63</v>
+      <c r="G2" s="1">
+        <v>31372</v>
       </c>
-      <c r="D2" s="6">
-        <v>41000782</v>
+      <c r="H2">
+        <v>9982140469</v>
       </c>
-      <c r="E2" s="7">
-        <v>31655710</v>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
       </c>
-      <c r="F2" s="9">
-        <v>42800</v>
+      <c r="K2" s="1">
+        <v>46352</v>
       </c>
-      <c r="G2" s="10">
-        <v>30635</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6">
-        <v>3184749980</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
       <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>49600123</v>
+      </c>
+      <c r="E3">
+        <v>123123123</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43320</v>
+      </c>
+      <c r="G3" s="1">
+        <v>31372</v>
+      </c>
+      <c r="H3">
+        <v>9982140469</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
+      <c r="K3" s="1">
+        <v>46352</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="6">
-        <v>41000786</v>
-      </c>
-      <c r="E3" s="7">
-        <v>31568063</v>
-      </c>
-      <c r="F3" s="9">
-        <v>42800</v>
-      </c>
-      <c r="G3" s="10">
-        <v>29600</v>
-      </c>
-      <c r="H3" s="6">
-        <v>3271835</v>
-      </c>
-      <c r="I3" s="6">
-        <v>3209760331</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="6" t="s">
+      <c r="M3" t="s">
         <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="6">
-        <v>41000861</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1115069862</v>
-      </c>
-      <c r="F4" s="9">
-        <v>42872</v>
-      </c>
-      <c r="G4" s="10">
-        <v>32402</v>
-      </c>
-      <c r="H4" s="6">
-        <v>3233575730</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="6">
-        <v>41000869</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1143971386</v>
-      </c>
-      <c r="F5" s="9">
-        <v>42872</v>
-      </c>
-      <c r="G5" s="10">
-        <v>34823</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6">
-        <v>3015906090</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="6">
-        <v>41000903</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1151946268</v>
-      </c>
-      <c r="F6" s="9">
-        <v>42898</v>
-      </c>
-      <c r="G6" s="10">
-        <v>33806</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6">
-        <v>3117850477</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="6">
-        <v>41000969</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1144175824</v>
-      </c>
-      <c r="F7" s="9">
-        <v>42949</v>
-      </c>
-      <c r="G7" s="10">
-        <v>34389</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6">
-        <v>3127622325</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="6">
-        <v>41000964</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1144147550</v>
-      </c>
-      <c r="F8" s="9">
-        <v>42949</v>
-      </c>
-      <c r="G8" s="10">
-        <v>33263</v>
-      </c>
-      <c r="H8" s="6">
-        <v>4877992</v>
-      </c>
-      <c r="I8" s="6">
-        <v>3137504991</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="6">
-        <v>41000972</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1151949372</v>
-      </c>
-      <c r="F9" s="9">
-        <v>42949</v>
-      </c>
-      <c r="G9" s="10">
-        <v>34099</v>
-      </c>
-      <c r="H9" s="6">
-        <v>6540301</v>
-      </c>
-      <c r="I9" s="6">
-        <v>3007207959</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="6">
-        <v>41001028</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1144050193</v>
-      </c>
-      <c r="F10" s="9">
-        <v>43010</v>
-      </c>
-      <c r="G10" s="10">
-        <v>33594</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6">
-        <v>3177436256</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="6">
-        <v>41001086</v>
-      </c>
-      <c r="E11" s="7">
-        <v>14638683</v>
-      </c>
-      <c r="F11" s="9">
-        <v>43111</v>
-      </c>
-      <c r="G11" s="10">
-        <v>30948</v>
-      </c>
-      <c r="H11" s="6">
-        <v>3341112</v>
-      </c>
-      <c r="I11" s="6">
-        <v>3008626231</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="6">
-        <v>41001094</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1144149271</v>
-      </c>
-      <c r="F12" s="9">
-        <v>43111</v>
-      </c>
-      <c r="G12" s="10">
-        <v>33306</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6">
-        <v>3146818497</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="6">
-        <v>41001093</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1143875138</v>
-      </c>
-      <c r="F13" s="9">
-        <v>43111</v>
-      </c>
-      <c r="G13" s="10">
-        <v>36041</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6">
-        <v>3184941045</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="6">
-        <v>41001146</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1107518087</v>
-      </c>
-      <c r="F14" s="9">
-        <v>43164</v>
-      </c>
-      <c r="G14" s="10">
-        <v>35939</v>
-      </c>
-      <c r="H14" s="6">
-        <v>3359693</v>
-      </c>
-      <c r="I14" s="6">
-        <v>3186576586</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="6">
-        <v>41001143</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1143974416</v>
-      </c>
-      <c r="F15" s="9">
-        <v>43164</v>
-      </c>
-      <c r="G15" s="10">
-        <v>34886</v>
-      </c>
-      <c r="H15" s="6">
-        <v>3922375</v>
-      </c>
-      <c r="I15" s="6">
-        <v>3106541523</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="6">
-        <v>41001176</v>
-      </c>
-      <c r="E16" s="7">
-        <v>1130599837</v>
-      </c>
-      <c r="F16" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G16" s="10">
-        <v>32267</v>
-      </c>
-      <c r="H16" s="6">
-        <v>4455922</v>
-      </c>
-      <c r="I16" s="6">
-        <v>3007300386</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="6">
-        <v>41001187</v>
-      </c>
-      <c r="E17" s="7">
-        <v>1151958983</v>
-      </c>
-      <c r="F17" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G17" s="10">
-        <v>35043</v>
-      </c>
-      <c r="H17" s="6">
-        <v>3837858</v>
-      </c>
-      <c r="I17" s="6">
-        <v>3154773906</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="17" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="6">
-        <v>41001178</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1095950835</v>
-      </c>
-      <c r="F18" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G18" s="10">
-        <v>35704</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6">
-        <v>3183699580</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="18" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="6">
-        <v>41001179</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1143830383</v>
-      </c>
-      <c r="F19" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G19" s="10">
-        <v>32837</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6">
-        <v>3207602837</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="19" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="6">
-        <v>41001172</v>
-      </c>
-      <c r="E20" s="7">
-        <v>549042</v>
-      </c>
-      <c r="F20" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G20" s="10">
-        <v>35003</v>
-      </c>
-      <c r="H20" s="6">
-        <v>3996399</v>
-      </c>
-      <c r="I20" s="6">
-        <v>3184012353</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="20" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="6">
-        <v>41001185</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1144146555</v>
-      </c>
-      <c r="F21" s="9">
-        <v>43201</v>
-      </c>
-      <c r="G21" s="10">
-        <v>33241</v>
-      </c>
-      <c r="H21" s="6">
-        <v>8828002</v>
-      </c>
-      <c r="I21" s="6">
-        <v>3134932123</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="21" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1127621942</v>
-      </c>
-      <c r="F22" s="9">
-        <v>43287</v>
-      </c>
-      <c r="G22" s="10">
-        <v>30159</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6">
-        <v>3158173509</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="22" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="6">
-        <v>41001244</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1144132795</v>
-      </c>
-      <c r="F23" s="9">
-        <v>43287</v>
-      </c>
-      <c r="G23" s="10">
-        <v>32861</v>
-      </c>
-      <c r="H23" s="6">
-        <v>3906762</v>
-      </c>
-      <c r="I23" s="6">
-        <v>3225904346</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="23" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="O32" s="1"/>
@@ -5975,12 +5052,121 @@
       <c r="J880" s="3"/>
       <c r="O880" s="1"/>
     </row>
+    <row r="881" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I881" s="3"/>
+      <c r="J881" s="3"/>
+      <c r="O881" s="1"/>
+    </row>
+    <row r="882" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I882" s="3"/>
+      <c r="J882" s="3"/>
+      <c r="O882" s="1"/>
+    </row>
+    <row r="883" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I883" s="3"/>
+      <c r="J883" s="3"/>
+      <c r="O883" s="1"/>
+    </row>
+    <row r="884" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I884" s="3"/>
+      <c r="J884" s="3"/>
+      <c r="O884" s="1"/>
+    </row>
+    <row r="885" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I885" s="3"/>
+      <c r="J885" s="3"/>
+      <c r="O885" s="1"/>
+    </row>
+    <row r="886" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I886" s="3"/>
+      <c r="J886" s="3"/>
+      <c r="O886" s="1"/>
+    </row>
+    <row r="887" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I887" s="3"/>
+      <c r="J887" s="3"/>
+      <c r="O887" s="1"/>
+    </row>
+    <row r="888" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I888" s="3"/>
+      <c r="J888" s="3"/>
+      <c r="O888" s="1"/>
+    </row>
+    <row r="889" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I889" s="3"/>
+      <c r="J889" s="3"/>
+      <c r="O889" s="1"/>
+    </row>
+    <row r="890" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I890" s="3"/>
+      <c r="J890" s="3"/>
+      <c r="O890" s="1"/>
+    </row>
+    <row r="891" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I891" s="3"/>
+      <c r="J891" s="3"/>
+      <c r="O891" s="1"/>
+    </row>
+    <row r="892" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I892" s="3"/>
+      <c r="J892" s="3"/>
+      <c r="O892" s="1"/>
+    </row>
+    <row r="893" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I893" s="3"/>
+      <c r="J893" s="3"/>
+      <c r="O893" s="1"/>
+    </row>
+    <row r="894" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I894" s="3"/>
+      <c r="J894" s="3"/>
+      <c r="O894" s="1"/>
+    </row>
+    <row r="895" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I895" s="3"/>
+      <c r="J895" s="3"/>
+      <c r="O895" s="1"/>
+    </row>
+    <row r="896" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I896" s="3"/>
+      <c r="J896" s="3"/>
+      <c r="O896" s="1"/>
+    </row>
+    <row r="897" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I897" s="3"/>
+      <c r="J897" s="3"/>
+      <c r="O897" s="1"/>
+    </row>
+    <row r="898" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I898" s="3"/>
+      <c r="J898" s="3"/>
+      <c r="O898" s="1"/>
+    </row>
+    <row r="899" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I899" s="3"/>
+      <c r="J899" s="3"/>
+      <c r="O899" s="1"/>
+    </row>
+    <row r="900" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I900" s="3"/>
+      <c r="J900" s="3"/>
+      <c r="O900" s="1"/>
+    </row>
+    <row r="901" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I901" s="3"/>
+      <c r="J901" s="3"/>
+      <c r="O901" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N879" xr:uid="{CDFC4FAB-8988-0148-974D-3D947605956E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N900" xr:uid="{CDFC4FAB-8988-0148-974D-3D947605956E}">
       <formula1>contratos</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{CE37D499-A427-D346-AEE1-B297A10DA969}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{0569F8B3-1914-E94F-AFC6-4A12CFDB1DB5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5989,23 +5175,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DF492-46FD-2341-8E22-5AE8562222D1}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>